<commit_message>
MISE A JOURS V2
</commit_message>
<xml_diff>
--- a/ToM/compVsMimic_Etude/EtudeFinale/ComportementPow.xlsx
+++ b/ToM/compVsMimic_Etude/EtudeFinale/ComportementPow.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
   <si>
     <t xml:space="preserve">H1</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t xml:space="preserve">Kevin Vs Arthur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simil.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neutre</t>
   </si>
   <si>
     <t xml:space="preserve">X__1 </t>
@@ -233,7 +242,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -330,10 +339,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -415,7 +420,7 @@
   <dimension ref="A1:H123"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F42:G49 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3638,7 +3643,7 @@
   <dimension ref="A1:H123"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="1" sqref="F42:G49 I2"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6863,7 +6868,7 @@
   <dimension ref="A1:H123"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A125" activeCellId="1" sqref="F42:G49 A125"/>
+      <selection pane="topLeft" activeCell="A125" activeCellId="0" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -10085,8 +10090,8 @@
   </sheetPr>
   <dimension ref="A1:J65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F42" activeCellId="0" sqref="F42:G49"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G37" activeCellId="0" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -10611,200 +10616,201 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G41" s="24"/>
+      <c r="A41" s="22"/>
+      <c r="B41" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G41" s="20"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="0" t="n">
+      <c r="B42" s="21" t="n">
         <v>1.942623</v>
       </c>
-      <c r="C42" s="0" t="n">
+      <c r="C42" s="21" t="n">
         <v>0.9297576</v>
       </c>
-      <c r="D42" s="0" t="n">
+      <c r="D42" s="21" t="n">
         <v>2.467213</v>
       </c>
-      <c r="E42" s="0" t="n">
+      <c r="E42" s="21" t="n">
         <v>1.114773</v>
       </c>
-      <c r="F42" s="0" t="n">
+      <c r="F42" s="21" t="n">
         <v>1.991803</v>
       </c>
-      <c r="G42" s="0" t="n">
+      <c r="G42" s="21" t="n">
         <v>0.9403349</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B43" s="0" t="n">
+      <c r="A43" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="21" t="n">
         <v>2.696721</v>
       </c>
-      <c r="C43" s="0" t="n">
+      <c r="C43" s="21" t="n">
         <v>1.149124</v>
       </c>
-      <c r="D43" s="0" t="n">
+      <c r="D43" s="21" t="n">
         <v>2.713115</v>
       </c>
-      <c r="E43" s="0" t="n">
+      <c r="E43" s="21" t="n">
         <v>1.063904</v>
       </c>
-      <c r="F43" s="0" t="n">
+      <c r="F43" s="21" t="n">
         <v>2.983607</v>
       </c>
-      <c r="G43" s="0" t="n">
+      <c r="G43" s="21" t="n">
         <v>1.083182</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B44" s="0" t="n">
+      <c r="B44" s="21" t="n">
         <v>3.803279</v>
       </c>
-      <c r="C44" s="0" t="n">
+      <c r="C44" s="21" t="n">
         <v>1.049513</v>
       </c>
-      <c r="D44" s="0" t="n">
+      <c r="D44" s="21" t="n">
         <v>3.704918</v>
       </c>
-      <c r="E44" s="0" t="n">
+      <c r="E44" s="21" t="n">
         <v>1.103627</v>
       </c>
-      <c r="F44" s="0" t="n">
+      <c r="F44" s="21" t="n">
         <v>3.811475</v>
       </c>
-      <c r="G44" s="0" t="n">
+      <c r="G44" s="21" t="n">
         <v>0.938893</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" s="0" t="n">
+      <c r="A45" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" s="21" t="n">
         <v>2.901639</v>
       </c>
-      <c r="C45" s="0" t="n">
+      <c r="C45" s="21" t="n">
         <v>1.235895</v>
       </c>
-      <c r="D45" s="0" t="n">
+      <c r="D45" s="21" t="n">
         <v>3.368852</v>
       </c>
-      <c r="E45" s="0" t="n">
+      <c r="E45" s="21" t="n">
         <v>1.038123</v>
       </c>
-      <c r="F45" s="0" t="n">
+      <c r="F45" s="21" t="n">
         <v>2.877049</v>
       </c>
-      <c r="G45" s="0" t="n">
+      <c r="G45" s="21" t="n">
         <v>1.117686</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B46" s="0" t="n">
+      <c r="B46" s="21" t="n">
         <v>2.237705</v>
       </c>
-      <c r="C46" s="0" t="n">
+      <c r="C46" s="21" t="n">
         <v>1.036948</v>
       </c>
-      <c r="D46" s="0" t="n">
+      <c r="D46" s="21" t="n">
         <v>3.090164</v>
       </c>
-      <c r="E46" s="0" t="n">
+      <c r="E46" s="21" t="n">
         <v>1.199202</v>
       </c>
-      <c r="F46" s="0" t="n">
+      <c r="F46" s="21" t="n">
         <v>2.278689</v>
       </c>
-      <c r="G46" s="0" t="n">
+      <c r="G46" s="21" t="n">
         <v>1.00628</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B47" s="0" t="n">
+      <c r="A47" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="21" t="n">
         <v>3.393443</v>
       </c>
-      <c r="C47" s="0" t="n">
+      <c r="C47" s="21" t="n">
         <v>1.032988</v>
       </c>
-      <c r="D47" s="0" t="n">
+      <c r="D47" s="21" t="n">
         <v>3.327869</v>
       </c>
-      <c r="E47" s="0" t="n">
+      <c r="E47" s="21" t="n">
         <v>1.063618</v>
       </c>
-      <c r="F47" s="0" t="n">
+      <c r="F47" s="21" t="n">
         <v>3.598361</v>
       </c>
-      <c r="G47" s="0" t="n">
+      <c r="G47" s="21" t="n">
         <v>1.00954</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B48" s="0" t="n">
+      <c r="B48" s="21" t="n">
         <v>3.081967</v>
       </c>
-      <c r="C48" s="0" t="n">
+      <c r="C48" s="21" t="n">
         <v>1.117776</v>
       </c>
-      <c r="D48" s="0" t="n">
+      <c r="D48" s="21" t="n">
         <v>3.229508</v>
       </c>
-      <c r="E48" s="0" t="n">
+      <c r="E48" s="21" t="n">
         <v>1.12659</v>
       </c>
-      <c r="F48" s="0" t="n">
+      <c r="F48" s="21" t="n">
         <v>3.02459</v>
       </c>
-      <c r="G48" s="0" t="n">
+      <c r="G48" s="21" t="n">
         <v>1.124212</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B49" s="0" t="n">
+      <c r="A49" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" s="21" t="n">
         <v>3.016393</v>
       </c>
-      <c r="C49" s="0" t="n">
+      <c r="C49" s="21" t="n">
         <v>1.020319</v>
       </c>
-      <c r="D49" s="0" t="n">
+      <c r="D49" s="21" t="n">
         <v>2.983607</v>
       </c>
-      <c r="E49" s="0" t="n">
+      <c r="E49" s="21" t="n">
         <v>1.090785</v>
       </c>
-      <c r="F49" s="0" t="n">
+      <c r="F49" s="21" t="n">
         <v>3.172131</v>
       </c>
-      <c r="G49" s="0" t="n">
+      <c r="G49" s="21" t="n">
         <v>1.103658</v>
       </c>
     </row>
@@ -10894,7 +10900,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F42:G49 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>